<commit_message>
Added error formula example
</commit_message>
<xml_diff>
--- a/2_Formulas_and_Functions/2_Functions_Intro/2_Basics_2.xlsx
+++ b/2_Formulas_and_Functions/2_Functions_Intro/2_Basics_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SaderPC\Documents\GitHub\Excel_Data_Analytics_Course\2_Formulas_and_Functions\2_Functions_Intro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54CD5C65-0AC2-4FA9-8A8F-C983493418C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CCE2A64-A2B9-46ED-872B-14B0AFDD4D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{52481452-F906-4392-9CAC-4FF33452D05D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{52481452-F906-4392-9CAC-4FF33452D05D}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -34,6 +34,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1262,10 +1284,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D0C29DB-E0EE-4D23-ADF3-5FE7700219C1}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1281,7 +1303,7 @@
     <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1310,7 +1332,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1339,7 +1361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1367,8 +1389,12 @@
       <c r="I3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L3" t="e">
+        <f>H2/0</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1393,8 +1419,12 @@
       <c r="I4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L4" t="e" cm="1">
+        <f t="array" ref="L4">SUM(A2:A3) + UNKNOWN</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1419,8 +1449,12 @@
       <c r="I5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L5" t="e">
+        <f>VLOOKUP("NonexistentValue", A2:A21, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -1445,8 +1479,12 @@
       <c r="I6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L6" t="e">
+        <f>SUM(A2:A3 B4:B5)</f>
+        <v>#NULL!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1471,8 +1509,12 @@
       <c r="I7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L7" t="e">
+        <f>SQRT(-1)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1497,8 +1539,12 @@
       <c r="I8" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L8" t="e">
+        <f>#REF!+A22</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1526,8 +1572,12 @@
       <c r="I9" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L9" t="e">
+        <f>A2 + "text"</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1553,7 +1603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1582,7 +1632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1611,7 +1661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -1640,7 +1690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1669,7 +1719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -1698,7 +1748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>56</v>
       </c>

</xml_diff>